<commit_message>
Se corrigió balance y estado de resultados.
</commit_message>
<xml_diff>
--- a/balance.xlsx
+++ b/balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oienh\Documents\R_UNIVERSITY_PROJECTS\5th_Semester\trabajo_finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D7AD3A-ADC0-410D-9D90-86B3856FFB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FAA0D3-9860-4A30-B50E-2C2355EDC9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="10980" windowHeight="13770" xr2:uid="{50824960-5866-452E-8A79-15478387813D}"/>
+    <workbookView xWindow="5400" yWindow="380" windowWidth="16200" windowHeight="9970" xr2:uid="{50824960-5866-452E-8A79-15478387813D}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Period Ending:</t>
   </si>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A52CFB-0E58-4378-B295-BEE1EBFCDE8D}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -835,7 +835,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1">
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -843,16 +843,16 @@
         <v>146791</v>
       </c>
       <c r="C3" s="2">
-        <v>131463</v>
+        <v>161580</v>
       </c>
       <c r="D3" s="2">
-        <v>133667</v>
+        <v>132733</v>
       </c>
       <c r="E3" s="11">
-        <v>133876</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="98">
+        <v>96334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -860,16 +860,16 @@
         <v>70026</v>
       </c>
       <c r="C4" s="3">
-        <v>58662</v>
+        <v>96049</v>
       </c>
       <c r="D4" s="3">
-        <v>60710</v>
+        <v>84396</v>
       </c>
       <c r="E4" s="13">
-        <v>66385</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="42">
+        <v>55021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="126">
+    <row r="6" spans="1:5">
       <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
@@ -894,16 +894,16 @@
         <v>53888</v>
       </c>
       <c r="C6" s="4">
-        <v>34947</v>
+        <v>36220</v>
       </c>
       <c r="D6" s="4">
-        <v>37478</v>
+        <v>42122</v>
       </c>
       <c r="E6" s="15">
-        <v>36393</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="112">
+        <v>36092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
@@ -911,16 +911,16 @@
         <v>16138</v>
       </c>
       <c r="C7" s="4">
-        <v>23715</v>
+        <v>59829</v>
       </c>
       <c r="D7" s="4">
-        <v>23232</v>
+        <v>42274</v>
       </c>
       <c r="E7" s="15">
-        <v>29992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="84">
+        <v>18929</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
@@ -928,16 +928,16 @@
         <v>42002</v>
       </c>
       <c r="C8" s="4">
-        <v>35930</v>
+        <v>32649</v>
       </c>
       <c r="D8" s="4">
-        <v>34597</v>
+        <v>24309</v>
       </c>
       <c r="E8" s="15">
-        <v>32313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="140">
+        <v>20540</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
@@ -945,16 +945,16 @@
         <v>33500</v>
       </c>
       <c r="C9" s="4">
-        <v>27700</v>
+        <v>25500</v>
       </c>
       <c r="D9" s="4">
-        <v>26500</v>
+        <v>24309</v>
       </c>
       <c r="E9" s="15">
-        <v>25100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="42">
+        <v>20540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
@@ -962,16 +962,16 @@
         <v>34405</v>
       </c>
       <c r="C10" s="4">
-        <v>36647</v>
+        <v>32640</v>
       </c>
       <c r="D10" s="4">
-        <v>38153</v>
+        <v>23795</v>
       </c>
       <c r="E10" s="15">
-        <v>34987</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="70">
+        <v>20497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="84.5" thickBot="1">
+    <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
@@ -996,13 +996,13 @@
         <v>358</v>
       </c>
       <c r="C12" s="4">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="D12" s="4">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="E12" s="15">
-        <v>191</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1">
@@ -1013,16 +1013,16 @@
         <v>462675</v>
       </c>
       <c r="C13" s="5">
-        <v>428362</v>
+        <v>420549</v>
       </c>
       <c r="D13" s="5">
-        <v>419728</v>
+        <v>321195</v>
       </c>
       <c r="E13" s="18">
-        <v>410767</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="98">
+        <v>225248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -1030,50 +1030,50 @@
         <v>252838</v>
       </c>
       <c r="C14" s="3">
-        <v>239228</v>
+        <v>216363</v>
       </c>
       <c r="D14" s="3">
-        <v>232136</v>
+        <v>150667</v>
       </c>
       <c r="E14" s="13">
-        <v>224629</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="140">
+        <v>97846</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="4">
         <v>349853</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="126">
+      <c r="C15" s="4">
+        <v>294882</v>
+      </c>
+      <c r="D15" s="4">
+        <v>211101</v>
+      </c>
+      <c r="E15" s="15">
+        <v>144821</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="4">
         <v>-97015</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="56">
+      <c r="C16" s="4">
+        <v>-78519</v>
+      </c>
+      <c r="D16" s="4">
+        <v>-60434</v>
+      </c>
+      <c r="E16" s="15">
+        <v>-46975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
@@ -1081,33 +1081,33 @@
         <v>20288</v>
       </c>
       <c r="C17" s="4">
-        <v>20168</v>
+        <v>15371</v>
       </c>
       <c r="D17" s="4">
-        <v>20195</v>
+        <v>15017</v>
       </c>
       <c r="E17" s="15">
-        <v>20229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="56">
+        <v>14754</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="4">
         <v>6097</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="84">
+      <c r="C18" s="4">
+        <v>5107</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4981</v>
+      </c>
+      <c r="E18" s="15">
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
@@ -1115,16 +1115,16 @@
         <v>2815</v>
       </c>
       <c r="C19" s="4">
-        <v>3331</v>
+        <v>4003</v>
       </c>
       <c r="D19" s="4">
-        <v>3168</v>
+        <v>3200</v>
       </c>
       <c r="E19" s="15">
-        <v>3957</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="98">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="16" t="s">
         <v>19</v>
       </c>
@@ -1132,16 +1132,16 @@
         <v>8502</v>
       </c>
       <c r="C20" s="4">
-        <v>8230</v>
-      </c>
-      <c r="D20" s="4">
-        <v>8097</v>
-      </c>
-      <c r="E20" s="15">
-        <v>7213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="98">
+        <v>7149</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="16" t="s">
         <v>20</v>
       </c>
@@ -1149,16 +1149,16 @@
         <v>33846</v>
       </c>
       <c r="C21" s="4">
-        <v>34172</v>
+        <v>18125</v>
       </c>
       <c r="D21" s="4">
-        <v>30562</v>
+        <v>14597</v>
       </c>
       <c r="E21" s="15">
-        <v>28076</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="56.5" thickBot="1">
+        <v>11586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1">
       <c r="A22" s="16" t="s">
         <v>21</v>
       </c>
@@ -1166,16 +1166,16 @@
         <v>8899</v>
       </c>
       <c r="C22" s="4">
-        <v>24656</v>
-      </c>
-      <c r="D22" s="4">
-        <v>26995</v>
-      </c>
-      <c r="E22" s="15">
-        <v>32857</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" thickBot="1">
+        <v>60062</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1">
       <c r="A23" s="17" t="s">
         <v>22</v>
       </c>
@@ -1183,16 +1183,16 @@
         <v>155393</v>
       </c>
       <c r="C23" s="5">
-        <v>140363</v>
+        <v>142266</v>
       </c>
       <c r="D23" s="5">
-        <v>140291</v>
+        <v>126385</v>
       </c>
       <c r="E23" s="18">
-        <v>139508</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="56">
+        <v>87812</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="12" t="s">
         <v>23</v>
       </c>
@@ -1200,16 +1200,16 @@
         <v>79600</v>
       </c>
       <c r="C24" s="3">
-        <v>67760</v>
+        <v>78664</v>
       </c>
       <c r="D24" s="3">
-        <v>71219</v>
+        <v>72539</v>
       </c>
       <c r="E24" s="13">
-        <v>68547</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="98">
+        <v>47183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="16" t="s">
         <v>24</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="70">
+    <row r="26" spans="1:5">
       <c r="A26" s="16" t="s">
         <v>6</v>
       </c>
@@ -1234,16 +1234,16 @@
         <v>32746</v>
       </c>
       <c r="C26" s="4">
-        <v>30591</v>
+        <v>28413</v>
       </c>
       <c r="D26" s="4">
-        <v>30071</v>
+        <v>42983</v>
       </c>
       <c r="E26" s="15">
-        <v>30961</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="126">
+        <v>31132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="16" t="s">
         <v>25</v>
       </c>
@@ -1251,16 +1251,16 @@
         <v>8000</v>
       </c>
       <c r="C27" s="4">
-        <v>12800</v>
-      </c>
-      <c r="D27" s="4">
-        <v>8435</v>
-      </c>
-      <c r="E27" s="15">
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="238">
+        <v>1043</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28">
       <c r="A28" s="16" t="s">
         <v>26</v>
       </c>
@@ -1268,16 +1268,16 @@
         <v>15120</v>
       </c>
       <c r="C28" s="4">
-        <v>16583</v>
+        <v>16119</v>
       </c>
       <c r="D28" s="4">
-        <v>17748</v>
+        <v>1155</v>
       </c>
       <c r="E28" s="15">
-        <v>16380</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="98.5" thickBot="1">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1">
       <c r="A29" s="16" t="s">
         <v>27</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>19927</v>
       </c>
       <c r="C29" s="4">
-        <v>12629</v>
+        <v>18027</v>
       </c>
       <c r="D29" s="4">
-        <v>12818</v>
+        <v>9708</v>
       </c>
       <c r="E29" s="15">
-        <v>12820</v>
+        <v>8190</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1">
@@ -1302,16 +1302,16 @@
         <v>316632</v>
       </c>
       <c r="C30" s="5">
-        <v>290873</v>
+        <v>282304</v>
       </c>
       <c r="D30" s="5">
-        <v>288326</v>
+        <v>227791</v>
       </c>
       <c r="E30" s="18">
-        <v>276766</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="84">
+        <v>163188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
@@ -1319,16 +1319,16 @@
         <v>85236</v>
       </c>
       <c r="C31" s="3">
-        <v>77214</v>
+        <v>70614</v>
       </c>
       <c r="D31" s="3">
-        <v>77478</v>
+        <v>49876</v>
       </c>
       <c r="E31" s="13">
-        <v>68441</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="84">
+        <v>40509</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="14" t="s">
         <v>30</v>
       </c>
@@ -1336,16 +1336,16 @@
         <v>73850</v>
       </c>
       <c r="C32" s="4">
-        <v>65619</v>
+        <v>54944</v>
       </c>
       <c r="D32" s="4">
-        <v>64853</v>
+        <v>31816</v>
       </c>
       <c r="E32" s="15">
-        <v>54356</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="210">
+        <v>23414</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28">
       <c r="A33" s="14" t="s">
         <v>31</v>
       </c>
@@ -1353,16 +1353,16 @@
         <v>11386</v>
       </c>
       <c r="C33" s="4">
-        <v>11595</v>
+        <v>15670</v>
       </c>
       <c r="D33" s="4">
-        <v>12625</v>
+        <v>18060</v>
       </c>
       <c r="E33" s="15">
-        <v>14085</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="98">
+        <v>17095</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="16" t="s">
         <v>32</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="84">
+    <row r="35" spans="1:5">
       <c r="A35" s="16" t="s">
         <v>33</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="56.5" thickBot="1">
+    <row r="36" spans="1:5" ht="15" thickBot="1">
       <c r="A36" s="16" t="s">
         <v>34</v>
       </c>
@@ -1404,16 +1404,16 @@
         <v>68003</v>
       </c>
       <c r="C36" s="4">
-        <v>60496</v>
+        <v>68381</v>
       </c>
       <c r="D36" s="4">
-        <v>62122</v>
+        <v>51530</v>
       </c>
       <c r="E36" s="15">
-        <v>58017</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="16.5" thickBot="1">
+        <v>34867</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1">
       <c r="A37" s="17" t="s">
         <v>35</v>
       </c>
@@ -1421,16 +1421,16 @@
         <v>146043</v>
       </c>
       <c r="C37" s="5">
-        <v>137489</v>
+        <v>138245</v>
       </c>
       <c r="D37" s="5">
-        <v>131402</v>
+        <v>93404</v>
       </c>
       <c r="E37" s="18">
-        <v>134001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="84">
+        <v>62060</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="56">
+    <row r="39" spans="1:5">
       <c r="A39" s="16" t="s">
         <v>16</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="70">
+    <row r="40" spans="1:5">
       <c r="A40" s="16" t="s">
         <v>37</v>
       </c>
@@ -1472,16 +1472,16 @@
         <v>108</v>
       </c>
       <c r="C40" s="4">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" s="4">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E40" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="84">
+    <row r="41" spans="1:5">
       <c r="A41" s="16" t="s">
         <v>38</v>
       </c>
@@ -1489,16 +1489,16 @@
         <v>75066</v>
       </c>
       <c r="C41" s="4">
-        <v>69419</v>
+        <v>55437</v>
       </c>
       <c r="D41" s="4">
-        <v>63871</v>
+        <v>42865</v>
       </c>
       <c r="E41" s="15">
-        <v>58793</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="98">
+        <v>33658</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="16" t="s">
         <v>39</v>
       </c>
@@ -1506,16 +1506,16 @@
         <v>83193</v>
       </c>
       <c r="C42" s="4">
-        <v>82915</v>
+        <v>85915</v>
       </c>
       <c r="D42" s="4">
-        <v>80043</v>
+        <v>52551</v>
       </c>
       <c r="E42" s="15">
-        <v>82071</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="126">
+        <v>31220</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="16" t="s">
         <v>40</v>
       </c>
@@ -1523,16 +1523,16 @@
         <v>-7837</v>
       </c>
       <c r="C43" s="4">
-        <v>-7837</v>
+        <v>-1837</v>
       </c>
       <c r="D43" s="4">
-        <v>-7837</v>
+        <v>-1837</v>
       </c>
       <c r="E43" s="15">
-        <v>-4503</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="98">
+        <v>-1837</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="16" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="98">
+    <row r="45" spans="1:5">
       <c r="A45" s="16" t="s">
         <v>42</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="70.5" thickBot="1">
+    <row r="46" spans="1:5" ht="15" thickBot="1">
       <c r="A46" s="16" t="s">
         <v>43</v>
       </c>
@@ -1574,16 +1574,16 @@
         <v>-4487</v>
       </c>
       <c r="C46" s="4">
-        <v>-7115</v>
+        <v>-1376</v>
       </c>
       <c r="D46" s="4">
-        <v>-4782</v>
+        <v>-180</v>
       </c>
       <c r="E46" s="15">
-        <v>-2365</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="24.5" thickBot="1">
+        <v>-986</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1">
       <c r="A47" s="19" t="s">
         <v>44</v>
       </c>
@@ -1591,16 +1591,16 @@
         <v>462675</v>
       </c>
       <c r="C47" s="6">
-        <v>428362</v>
+        <v>420549</v>
       </c>
       <c r="D47" s="6">
-        <v>419728</v>
+        <v>321195</v>
       </c>
       <c r="E47" s="20">
-        <v>410767</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="32.5" thickBot="1">
+        <v>225248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1">
       <c r="A48" s="19" t="s">
         <v>45</v>
       </c>
@@ -1608,16 +1608,16 @@
         <v>10242</v>
       </c>
       <c r="C48" s="6">
-        <v>10198</v>
+        <v>10180</v>
       </c>
       <c r="D48" s="6">
-        <v>10183</v>
+        <v>10060</v>
       </c>
       <c r="E48" s="20">
-        <v>10170.799999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="32.5" thickBot="1">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1">
       <c r="A49" s="21" t="s">
         <v>46</v>
       </c>
@@ -1639,5 +1639,6 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>